<commit_message>
29032021 -correcion en la generacion del reporte de contraloria -se agrega nueva condicion a reporte cdc finanzas
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/CDCFinanzas.xlsx
+++ b/App.Web/App_Data/CDCFinanzas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GestionProcesos\Reportes\Cometidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GestionProcesos\SourceNew\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6780CE1-18D4-43D4-BE41-9271AA21CF05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5B3740-115F-48B2-8369-DCB95E92BC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -73,16 +73,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,7 +110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -404,7 +396,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>